<commit_message>
added last six data
</commit_message>
<xml_diff>
--- a/Divisions/B1.xlsx
+++ b/Divisions/B1.xlsx
@@ -1,23 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\Rsoccer\Divisions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11280" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Table" r:id="rId3" sheetId="1"/>
-    <sheet name="Form" r:id="rId4" sheetId="2"/>
-    <sheet name="Goals scored" r:id="rId5" sheetId="3"/>
-    <sheet name="Goals conceded" r:id="rId6" sheetId="4"/>
-    <sheet name="Total Goals form" r:id="rId7" sheetId="5"/>
-    <sheet name="Goal totals v2" r:id="rId8" sheetId="6"/>
+    <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Form" sheetId="2" r:id="rId2"/>
+    <sheet name="Goals scored" sheetId="3" r:id="rId3"/>
+    <sheet name="Goals conceded" sheetId="4" r:id="rId4"/>
+    <sheet name="Total Goals form" sheetId="5" r:id="rId5"/>
+    <sheet name="Goal totals v2" sheetId="6" r:id="rId6"/>
+    <sheet name="L6" sheetId="7" r:id="rId7"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10520" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10614" uniqueCount="340">
   <si>
     <t>Team</t>
   </si>
@@ -809,16 +817,243 @@
   </si>
   <si>
     <t>3.3529</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>Goals scored</t>
+  </si>
+  <si>
+    <t>Goals conceded</t>
+  </si>
+  <si>
+    <t>Total Goals</t>
+  </si>
+  <si>
+    <t>Anderlecht,W D W W W W</t>
+  </si>
+  <si>
+    <t>Antwerp,L W W L W W</t>
+  </si>
+  <si>
+    <t>Beerschot VA,D W L W L L</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,W L L W W D</t>
+  </si>
+  <si>
+    <t>Charleroi,D D D L L L</t>
+  </si>
+  <si>
+    <t>Club Brugge,D W L W L W</t>
+  </si>
+  <si>
+    <t>Eupen,W D W L L W</t>
+  </si>
+  <si>
+    <t>Genk,W W D W W L</t>
+  </si>
+  <si>
+    <t>Gent,W L W L W W</t>
+  </si>
+  <si>
+    <t>Kortrijk,L L L L W L</t>
+  </si>
+  <si>
+    <t>Mechelen,L D D L W W</t>
+  </si>
+  <si>
+    <t>Mouscron,D W L D L L</t>
+  </si>
+  <si>
+    <t>Oostende,W L W L W D</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,W D D L L L</t>
+  </si>
+  <si>
+    <t>St Truiden,L D W W L L</t>
+  </si>
+  <si>
+    <t>Standard,L L D W W W</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,L L W L L W</t>
+  </si>
+  <si>
+    <t>Waregem,W L L W L L</t>
+  </si>
+  <si>
+    <t>Anderlecht,3 1 4 4 2 1</t>
+  </si>
+  <si>
+    <t>Antwerp,0 4 2 1 3 3</t>
+  </si>
+  <si>
+    <t>Beerschot VA,2 2 1 2 1 0</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,2 0 0 2 3 1</t>
+  </si>
+  <si>
+    <t>Charleroi,0 1 1 1 0 2</t>
+  </si>
+  <si>
+    <t>Club Brugge,1 4 0 2 1 4</t>
+  </si>
+  <si>
+    <t>Eupen,2 3 2 1 0 3</t>
+  </si>
+  <si>
+    <t>Genk,2 2 2 3 4 2</t>
+  </si>
+  <si>
+    <t>Gent,1 0 1 1 4 7</t>
+  </si>
+  <si>
+    <t>Kortrijk,1 2 0 1 4 1</t>
+  </si>
+  <si>
+    <t>Mechelen,0 1 2 1 4 4</t>
+  </si>
+  <si>
+    <t>Mouscron,2 1 0 1 2 2</t>
+  </si>
+  <si>
+    <t>Oostende,2 0 1 0 2 1</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,2 3 2 2 0 1</t>
+  </si>
+  <si>
+    <t>St Truiden,0 0 2 4 0 0</t>
+  </si>
+  <si>
+    <t>Standard,1 0 2 2 4 3</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,0 1 2 2 3 2</t>
+  </si>
+  <si>
+    <t>Waregem,2 0 1 2 2 2</t>
+  </si>
+  <si>
+    <t>Anderlecht,1 1 1 1 1 0</t>
+  </si>
+  <si>
+    <t>Antwerp,2 2 0 4 2 2</t>
+  </si>
+  <si>
+    <t>Beerschot VA,2 1 2 1 2 3</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,0 2 1 1 0 1</t>
+  </si>
+  <si>
+    <t>Charleroi,0 1 1 2 4 3</t>
+  </si>
+  <si>
+    <t>Club Brugge,1 0 2 1 2 2</t>
+  </si>
+  <si>
+    <t>Eupen,0 3 0 2 4 2</t>
+  </si>
+  <si>
+    <t>Genk,1 0 2 2 0 3</t>
+  </si>
+  <si>
+    <t>Gent,0 4 0 2 0 2</t>
+  </si>
+  <si>
+    <t>Kortrijk,2 4 2 2 3 4</t>
+  </si>
+  <si>
+    <t>Mechelen,2 1 2 2 2 1</t>
+  </si>
+  <si>
+    <t>Mouscron,2 0 1 1 3 4</t>
+  </si>
+  <si>
+    <t>Oostende,0 1 0 2 1 1</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,0 3 2 3 3 2</t>
+  </si>
+  <si>
+    <t>St Truiden,2 0 1 2 4 1</t>
+  </si>
+  <si>
+    <t>Standard,3 1 2 1 0 0</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,2 2 0 4 4 1</t>
+  </si>
+  <si>
+    <t>Waregem,1 3 4 1 4 7</t>
+  </si>
+  <si>
+    <t>Anderlecht,4 2 5 5 3 1</t>
+  </si>
+  <si>
+    <t>Antwerp,2 6 2 5 5 5</t>
+  </si>
+  <si>
+    <t>Beerschot VA,4 3 3 3 3 3</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,2 2 1 3 3 2</t>
+  </si>
+  <si>
+    <t>Charleroi,0 2 2 3 4 5</t>
+  </si>
+  <si>
+    <t>Club Brugge,2 4 2 3 3 6</t>
+  </si>
+  <si>
+    <t>Eupen,2 6 2 3 4 5</t>
+  </si>
+  <si>
+    <t>Genk,3 2 4 5 4 5</t>
+  </si>
+  <si>
+    <t>Gent,1 4 1 3 4 9</t>
+  </si>
+  <si>
+    <t>Kortrijk,3 6 2 3 7 5</t>
+  </si>
+  <si>
+    <t>Mechelen,2 2 4 3 6 5</t>
+  </si>
+  <si>
+    <t>Mouscron,4 1 1 2 5 6</t>
+  </si>
+  <si>
+    <t>Oostende,2 1 1 2 3 2</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,2 6 4 5 3 3</t>
+  </si>
+  <si>
+    <t>St Truiden,2 0 3 6 4 1</t>
+  </si>
+  <si>
+    <t>Standard,4 1 4 3 4 3</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,2 3 2 6 7 3</t>
+  </si>
+  <si>
+    <t>Waregem,3 3 5 3 6 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -830,7 +1065,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -848,19 +1083,292 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +1397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -921,7 +1429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -953,7 +1461,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -985,7 +1493,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1525,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1049,7 +1557,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1589,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1113,7 +1621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1145,7 +1653,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1177,7 +1685,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1717,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1241,7 +1749,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1781,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1305,7 +1813,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1337,7 +1845,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +1877,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1401,7 +1909,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1433,7 +1941,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1466,20 +1974,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DZ19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:130" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>91</v>
       </c>
@@ -1868,7 +2375,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2260,7 +2767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2652,7 +3159,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3044,7 +3551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3436,7 +3943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3828,7 +4335,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -4220,7 +4727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -4612,7 +5119,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -5004,7 +5511,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -5396,7 +5903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -5788,7 +6295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -6180,7 +6687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -6572,7 +7079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -6964,7 +7471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -7356,7 +7863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -7748,7 +8255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -8140,7 +8647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -8532,7 +9039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -8925,20 +9432,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DZ19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:130" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>91</v>
       </c>
@@ -9327,7 +9833,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -9719,7 +10225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -10111,7 +10617,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -10503,7 +11009,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -10895,7 +11401,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -11287,7 +11793,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -11679,7 +12185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -12071,7 +12577,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -12463,7 +12969,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -12855,7 +13361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -13247,7 +13753,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -13639,7 +14145,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -14031,7 +14537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -14423,7 +14929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -14815,7 +15321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -15207,7 +15713,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -15599,7 +16105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -15991,7 +16497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -16384,20 +16890,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DZ19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:130" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>91</v>
       </c>
@@ -16786,7 +17291,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -17178,7 +17683,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -17570,7 +18075,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -17962,7 +18467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -18354,7 +18859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -18746,7 +19251,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -19138,7 +19643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -19530,7 +20035,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -19922,7 +20427,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -20314,7 +20819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -20706,7 +21211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -21098,7 +21603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -21490,7 +21995,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -21882,7 +22387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -22274,7 +22779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -22666,7 +23171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -23058,7 +23563,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -23450,7 +23955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -23843,20 +24348,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DZ19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:130" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>91</v>
       </c>
@@ -24245,7 +24749,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -24637,7 +25141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -25029,7 +25533,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -25421,7 +25925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -25813,7 +26317,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -26205,7 +26709,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -26597,7 +27101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -26989,7 +27493,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -27381,7 +27885,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -27773,7 +28277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -28165,7 +28669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -28557,7 +29061,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -28949,7 +29453,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -29341,7 +29845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -29733,7 +30237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -30125,7 +30629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -30517,7 +31021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -30909,7 +31413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:130" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -31302,20 +31806,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1"/>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>29</v>
       </c>
@@ -31386,7 +31889,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -31460,7 +31963,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -31534,7 +32037,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -31608,7 +32111,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -31682,7 +32185,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -31756,7 +32259,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -31830,7 +32333,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -31904,7 +32407,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -31978,7 +32481,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -32052,7 +32555,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -32126,7 +32629,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -32200,7 +32703,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -32274,7 +32777,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -32348,7 +32851,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -32422,7 +32925,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -32496,7 +32999,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -32570,7 +33073,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -32644,7 +33147,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -32719,6 +33222,347 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D6" t="s">
+        <v>308</v>
+      </c>
+      <c r="E6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" t="s">
+        <v>310</v>
+      </c>
+      <c r="E8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" t="s">
+        <v>312</v>
+      </c>
+      <c r="E10" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" t="s">
+        <v>295</v>
+      </c>
+      <c r="D11" t="s">
+        <v>313</v>
+      </c>
+      <c r="E11" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>278</v>
+      </c>
+      <c r="C12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" t="s">
+        <v>314</v>
+      </c>
+      <c r="E12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" t="s">
+        <v>315</v>
+      </c>
+      <c r="E13" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" t="s">
+        <v>316</v>
+      </c>
+      <c r="E14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" t="s">
+        <v>317</v>
+      </c>
+      <c r="E15" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
+        <v>300</v>
+      </c>
+      <c r="D16" t="s">
+        <v>318</v>
+      </c>
+      <c r="E16" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" t="s">
+        <v>301</v>
+      </c>
+      <c r="D17" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" t="s">
+        <v>321</v>
+      </c>
+      <c r="E19" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added sum of goals scored,conceded and totals in last six
</commit_message>
<xml_diff>
--- a/Divisions/B1.xlsx
+++ b/Divisions/B1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard.000\gitboyzorro5\Rsoccer\Divisions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\Rsoccer\Divisions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11940" windowHeight="4500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" tabRatio="731" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="Shots Analysis" sheetId="7" r:id="rId7"/>
     <sheet name="L6" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10783" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10801" uniqueCount="480">
   <si>
     <t>Team</t>
   </si>
@@ -1198,274 +1198,274 @@
     <t>Team against</t>
   </si>
   <si>
-    <t>Anderlecht,D W D D W W D L D W W D L D D W W L W L L W D D D W D L W D W W W W</t>
-  </si>
-  <si>
-    <t>Antwerp,D L W L W D W W W W L D D W L L L W W L W W L W W W D D L W W L W W</t>
-  </si>
-  <si>
-    <t>Beerschot VA,W W W L W L W L W L W D W W L L L L D D L L W D W L L W D W L W L L</t>
-  </si>
-  <si>
-    <t>Cercle Brugge,L W W L L W L W W L L W L L L L L L L D L L W L L L D W W L L W W D</t>
-  </si>
-  <si>
-    <t>Charleroi,W W W W W W D L L W D L L L D W W W L L L L L D W D D L D D D L L L</t>
-  </si>
-  <si>
-    <t>Club Brugge,L W L W W W W W D L D W W D W W W L W W W W W W W W W W D W L W L W</t>
-  </si>
-  <si>
-    <t>Eupen,D L D D W D D L W L D D W D W L L L W D W W L L D D L D W D W L L W</t>
-  </si>
-  <si>
-    <t>Genk,W D D L L W D D W W W W W W W L W D W L L D L W D L L L W W D W W L</t>
-  </si>
-  <si>
-    <t>Gent,L L L W L W L W L L W D W L L W W W L D L D W D D D W D W L W L W W</t>
-  </si>
-  <si>
-    <t>Kortrijk,L W D W W L L D W L D D L W D L W L W W L L L D L W L W L L L L W L</t>
-  </si>
-  <si>
-    <t>Mechelen,D W L L L L W L L D D W L D D L L W W W W L W W D W W D L D D L W W</t>
-  </si>
-  <si>
-    <t>Mouscron,D L D L L L D L L L W D W L L W D W L L W D W D D L L L D W L D L L</t>
-  </si>
-  <si>
-    <t>Oostende,L L D D W W D W W L L D L L W W L W W D W L W D L W W D W L W L W D</t>
-  </si>
-  <si>
-    <t>Oud-Heverlee Leuven,D D L W W L W W D W L D L W W W D L L W L W L D L D W L W D D L L L</t>
-  </si>
-  <si>
-    <t>St Truiden,W L D D L L L D L W L D D L L L W W W L W W L D W L L D L D W W L L</t>
-  </si>
-  <si>
-    <t>Standard,W W D W L W D W D L W D D D D L L L L W W W W D L D D L L L D W W W</t>
-  </si>
-  <si>
-    <t>Waasland-Beveren,W L L L L L L D L D L W D W W W L L D L L D D L L L W D L L W L L W</t>
-  </si>
-  <si>
-    <t>Waregem,L L W W L L D L L L D W L W D W L W W W W L L L W D W W W L L W L L</t>
-  </si>
-  <si>
-    <t>Anderlecht,2 3 1 2 2 4 1 0 2 3 1 1 1 0 2 1 2 0 2 0 0 3 0 1 0 2 0 0 3 1 4 4 2 1</t>
-  </si>
-  <si>
-    <t>Antwerp,1 1 1 0 3 2 3 4 3 3 0 1 1 3 2 0 0 3 2 0 1 1 1 2 3 2 1 0 0 4 2 1 3 3</t>
-  </si>
-  <si>
-    <t>Beerschot VA,2 3 1 0 5 1 3 1 6 2 4 5 2 3 0 1 0 0 1 1 0 1 3 0 1 1 1 2 2 2 1 2 1 0</t>
-  </si>
-  <si>
-    <t>Cercle Brugge,0 2 3 0 0 3 1 2 5 0 1 2 1 1 1 0 3 0 1 1 0 0 2 1 0 0 0 2 2 0 0 2 3 1</t>
-  </si>
-  <si>
-    <t>Charleroi,1 1 3 2 2 3 1 1 1 3 3 0 1 0 0 2 4 1 1 2 0 0 2 1 3 1 1 1 0 1 1 1 0 2</t>
-  </si>
-  <si>
-    <t>Club Brugge,0 4 0 2 4 6 2 3 1 1 2 3 1 0 1 2 3 0 3 2 3 2 3 2 3 2 3 3 1 4 0 2 1 4</t>
-  </si>
-  <si>
-    <t>Eupen,1 0 0 1 2 2 1 1 2 0 1 2 3 1 1 0 2 1 2 1 2 3 0 0 1 2 0 1 2 3 2 1 0 3</t>
-  </si>
-  <si>
-    <t>Genk,2 1 0 1 2 3 2 1 2 2 4 2 4 5 4 0 2 1 4 1 0 1 2 3 0 1 1 1 2 2 2 3 4 2</t>
-  </si>
-  <si>
-    <t>Gent,1 1 0 1 1 1 2 5 2 1 4 1 1 0 1 2 3 1 0 1 0 1 3 1 0 2 4 1 1 0 1 1 4 7</t>
-  </si>
-  <si>
-    <t>Kortrijk,1 2 0 1 3 1 1 0 2 1 1 5 0 3 0 0 2 0 1 2 1 0 1 0 1 3 1 2 1 2 0 1 4 1</t>
-  </si>
-  <si>
-    <t>Mechelen,2 1 2 0 0 1 2 1 1 2 3 2 2 1 2 2 0 2 2 3 1 0 3 3 0 1 2 1 0 1 2 1 4 4</t>
-  </si>
-  <si>
-    <t>Mouscron,1 0 1 0 0 0 1 0 0 1 2 0 3 0 0 3 2 1 1 0 2 1 2 1 1 0 0 1 2 1 0 1 2 2</t>
-  </si>
-  <si>
-    <t>Oostende,1 0 0 2 1 3 2 3 3 0 1 1 0 1 2 1 1 2 3 1 2 1 2 2 1 3 3 1 2 0 1 0 2 1</t>
-  </si>
-  <si>
-    <t>Oud-Heverlee Leuven,1 1 1 3 1 1 3 2 2 2 2 2 2 2 2 3 2 1 1 1 1 3 0 1 0 1 3 0 2 3 2 2 0 1</t>
-  </si>
-  <si>
-    <t>St Truiden,2 1 0 1 2 0 0 0 3 2 1 2 1 2 0 1 2 2 1 1 3 2 0 1 3 1 1 0 0 0 2 4 0 0</t>
-  </si>
-  <si>
-    <t>Standard,1 2 0 3 0 2 2 2 1 0 1 1 2 0 2 1 1 0 1 3 1 4 3 2 1 1 1 2 1 0 2 2 4 3</t>
-  </si>
-  <si>
-    <t>Waasland-Beveren,3 1 1 1 1 2 2 1 1 1 0 2 1 2 2 3 0 0 1 1 1 1 0 2 2 0 1 1 0 1 2 2 3 2</t>
-  </si>
-  <si>
-    <t>Waregem,1 1 4 1 0 0 2 1 1 0 1 3 1 3 2 1 0 1 3 1 5 2 0 2 2 1 2 3 2 0 1 2 2 2</t>
-  </si>
-  <si>
-    <t>Anderlecht,2 1 1 2 0 2 1 3 2 1 0 1 2 0 2 0 1 1 0 1 2 0 0 1 0 1 0 2 1 1 1 1 1 0</t>
-  </si>
-  <si>
-    <t>Antwerp,1 2 0 2 2 2 1 1 1 2 1 1 1 2 4 2 1 0 1 3 0 0 2 0 2 1 1 0 2 2 0 4 2 2</t>
-  </si>
-  <si>
-    <t>Beerschot VA,1 1 0 3 2 3 2 5 3 3 2 5 1 2 1 3 2 1 1 1 3 3 0 0 0 2 2 1 2 1 2 1 2 3</t>
-  </si>
-  <si>
-    <t>Cercle Brugge,1 1 2 1 2 0 2 1 2 3 3 0 2 5 2 1 4 1 2 1 1 1 1 2 3 1 0 1 0 2 1 1 0 1</t>
-  </si>
-  <si>
-    <t>Charleroi,0 0 1 0 0 1 1 2 2 0 3 1 3 2 0 1 3 0 2 3 1 3 3 1 1 1 1 2 0 1 1 2 4 3</t>
-  </si>
-  <si>
-    <t>Club Brugge,1 0 1 1 1 0 1 0 1 2 2 1 0 0 0 0 0 1 0 1 0 1 2 1 1 0 0 0 1 0 2 1 2 2</t>
-  </si>
-  <si>
-    <t>Eupen,1 4 0 1 1 2 1 2 0 4 1 2 1 1 0 3 3 4 1 1 0 1 3 2 1 2 1 1 0 3 0 2 4 2</t>
-  </si>
-  <si>
-    <t>Genk,1 1 0 2 5 1 2 1 1 1 0 1 1 1 2 1 0 1 1 2 2 1 3 2 0 2 3 2 1 0 2 2 0 3</t>
-  </si>
-  <si>
-    <t>Gent,2 2 1 0 2 0 3 1 5 2 1 1 0 3 2 1 0 0 1 1 1 1 0 1 0 2 0 1 0 4 0 2 0 2</t>
-  </si>
-  <si>
-    <t>Kortrijk,3 1 0 0 0 2 3 0 1 3 1 5 1 1 0 3 1 2 0 1 2 2 2 0 3 0 3 0 2 4 2 2 3 4</t>
-  </si>
-  <si>
-    <t>Mechelen,2 0 3 1 1 3 0 4 2 2 3 1 3 1 2 3 3 1 1 0 0 4 0 2 0 0 1 1 2 1 2 2 2 1</t>
-  </si>
-  <si>
-    <t>Mouscron,1 1 1 1 3 1 1 3 2 4 1 0 2 2 2 1 2 0 2 1 0 1 0 1 1 3 4 2 2 0 1 1 3 4</t>
-  </si>
-  <si>
-    <t>Oostende,2 1 0 2 0 1 2 0 0 1 3 1 2 3 1 0 2 1 2 1 1 2 1 2 2 1 1 1 0 1 0 2 1 1</t>
-  </si>
-  <si>
-    <t>Oud-Heverlee Leuven,1 1 3 1 0 3 2 1 2 1 4 2 3 1 0 0 2 2 2 0 3 2 3 1 1 1 1 3 0 3 2 3 3 2</t>
-  </si>
-  <si>
-    <t>St Truiden,1 3 0 1 3 3 2 0 6 0 2 2 1 3 1 2 0 1 0 2 1 0 2 1 0 3 2 0 2 0 1 2 4 1</t>
-  </si>
-  <si>
-    <t>Standard,0 1 0 0 1 1 2 1 1 2 0 1 2 0 2 2 2 1 2 1 0 0 2 2 3 1 1 3 3 1 2 1 0 0</t>
-  </si>
-  <si>
-    <t>Waasland-Beveren,1 2 4 3 4 4 3 1 4 1 2 0 1 0 0 2 3 3 1 3 5 1 0 3 3 2 0 1 2 2 0 4 4 1</t>
-  </si>
-  <si>
-    <t>Waregem,2 3 1 0 2 6 2 2 3 3 1 1 2 0 2 0 2 0 2 0 1 3 3 3 1 1 1 2 1 3 4 1 4 7</t>
-  </si>
-  <si>
-    <t>Anderlecht,4 4 2 4 2 6 2 3 4 4 1 2 3 0 4 1 3 1 2 1 2 3 0 2 0 3 0 2 4 2 5 5 3 1</t>
-  </si>
-  <si>
-    <t>Antwerp,2 3 1 2 5 4 4 5 4 5 1 2 2 5 6 2 1 3 3 3 1 1 3 2 5 3 2 0 2 6 2 5 5 5</t>
-  </si>
-  <si>
-    <t>Beerschot VA,3 4 1 3 7 4 5 6 9 5 6 10 3 5 1 4 2 1 2 2 3 4 3 0 1 3 3 3 4 3 3 3 3 3</t>
-  </si>
-  <si>
-    <t>Cercle Brugge,1 3 5 1 2 3 3 3 7 3 4 2 3 6 3 1 7 1 3 2 1 1 3 3 3 1 0 3 2 2 1 3 3 2</t>
-  </si>
-  <si>
-    <t>Charleroi,1 1 4 2 2 4 2 3 3 3 6 1 4 2 0 3 7 1 3 5 1 3 5 2 4 2 2 3 0 2 2 3 4 5</t>
-  </si>
-  <si>
-    <t>Club Brugge,1 4 1 3 5 6 3 3 2 3 4 4 1 0 1 2 3 1 3 3 3 3 5 3 4 2 3 3 2 4 2 3 3 6</t>
-  </si>
-  <si>
-    <t>Eupen,2 4 0 2 3 4 2 3 2 4 2 4 4 2 1 3 5 5 3 2 2 4 3 2 2 4 1 2 2 6 2 3 4 5</t>
-  </si>
-  <si>
-    <t>Genk,3 2 0 3 7 4 4 2 3 3 4 3 5 6 6 1 2 2 5 3 2 2 5 5 0 3 4 3 3 2 4 5 4 5</t>
-  </si>
-  <si>
-    <t>Gent,3 3 1 1 3 1 5 6 7 3 5 2 1 3 3 3 3 1 1 2 1 2 3 2 0 4 4 2 1 4 1 3 4 9</t>
-  </si>
-  <si>
-    <t>Kortrijk,4 3 0 1 3 3 4 0 3 4 2 10 1 4 0 3 3 2 1 3 3 2 3 0 4 3 4 2 3 6 2 3 7 5</t>
-  </si>
-  <si>
-    <t>Mechelen,4 1 5 1 1 4 2 5 3 4 6 3 5 2 4 5 3 3 3 3 1 4 3 5 0 1 3 2 2 2 4 3 6 5</t>
-  </si>
-  <si>
-    <t>Mouscron,2 1 2 1 3 1 2 3 2 5 3 0 5 2 2 4 4 1 3 1 2 2 2 2 2 3 4 3 4 1 1 2 5 6</t>
-  </si>
-  <si>
-    <t>Oostende,3 1 0 4 1 4 4 3 3 1 4 2 2 4 3 1 3 3 5 2 3 3 3 4 3 4 4 2 2 1 1 2 3 2</t>
-  </si>
-  <si>
-    <t>Oud-Heverlee Leuven,2 2 4 4 1 4 5 3 4 3 6 4 5 3 2 3 4 3 3 1 4 5 3 2 1 2 4 3 2 6 4 5 3 3</t>
-  </si>
-  <si>
-    <t>St Truiden,3 4 0 2 5 3 2 0 9 2 3 4 2 5 1 3 2 3 1 3 4 2 2 2 3 4 3 0 2 0 3 6 4 1</t>
-  </si>
-  <si>
-    <t>Standard,1 3 0 3 1 3 4 3 2 2 1 2 4 0 4 3 3 1 3 4 1 4 5 4 4 2 2 5 4 1 4 3 4 3</t>
-  </si>
-  <si>
-    <t>Waasland-Beveren,4 3 5 4 5 6 5 2 5 2 2 2 2 2 2 5 3 3 2 4 6 2 0 5 5 2 1 2 2 3 2 6 7 3</t>
-  </si>
-  <si>
-    <t>Waregem,3 4 5 1 2 6 4 3 4 3 2 4 3 3 4 1 2 1 5 1 6 5 3 5 3 2 3 5 3 3 5 3 6 9</t>
-  </si>
-  <si>
-    <t>Anderlecht,Mechelen St Truiden Mouscron Oostende Cercle Brugge Waasland-Beveren Eupen Club Brugge Oud-Heverlee Leuven Kortrijk Antwerp Gent Beerschot VA Standard Waregem Genk Oostende Charleroi Beerschot VA Oud-Heverlee Leuven Eupen Charleroi Waasland-Beveren Mouscron Gent Genk Cercle Brugge Kortrijk Standard Mechelen Waregem Antwerp Club Brugge St Truiden</t>
-  </si>
-  <si>
-    <t>Antwerp,Mouscron Cercle Brugge Gent Charleroi St Truiden Eupen Kortrijk Mechelen Waregem Beerschot VA Anderlecht Standard Oostende Oud-Heverlee Leuven Genk Club Brugge Waregem Waasland-Beveren Charleroi Mechelen Gent Cercle Brugge Oostende Eupen Waasland-Beveren Beerschot VA Standard St Truiden Oud-Heverlee Leuven Kortrijk Club Brugge Anderlecht Mouscron Genk</t>
-  </si>
-  <si>
-    <t>Beerschot VA,Oostende Waregem Club Brugge Standard Genk Charleroi Waasland-Beveren Gent St Truiden Antwerp Oud-Heverlee Leuven Kortrijk Anderlecht Mechelen Eupen Mouscron Anderlecht St Truiden Gent Cercle Brugge Club Brugge Eupen Waregem Kortrijk Oud-Heverlee Leuven Antwerp Mechelen Genk Mouscron Waasland-Beveren Cercle Brugge Charleroi Oostende Standard</t>
-  </si>
-  <si>
-    <t>Cercle Brugge,Standard Antwerp Mechelen Kortrijk Anderlecht St Truiden Club Brugge Eupen Gent Charleroi Waregem Waasland-Beveren Mouscron Genk Oud-Heverlee Leuven Oostende Charleroi Waregem Eupen Beerschot VA Standard Antwerp Kortrijk Club Brugge St Truiden Mechelen Anderlecht Mouscron Waasland-Beveren Genk Gent Beerschot VA Oud-Heverlee Leuven Oostende</t>
-  </si>
-  <si>
-    <t>Charleroi,Club Brugge Oostende Oud-Heverlee Leuven Antwerp Waregem Beerschot VA Mouscron Standard Genk Cercle Brugge Mechelen Gent Eupen Waasland-Beveren Kortrijk St Truiden Cercle Brugge Anderlecht Antwerp Oostende Mechelen Anderlecht Standard Oud-Heverlee Leuven Kortrijk Waregem Waasland-Beveren Genk St Truiden Club Brugge Mouscron Beerschot VA Gent Eupen</t>
-  </si>
-  <si>
-    <t>Club Brugge,Charleroi Eupen Beerschot VA Genk Waasland-Beveren Waregem Cercle Brugge Anderlecht Standard Oud-Heverlee Leuven Mechelen Oostende Kortrijk Mouscron St Truiden Antwerp Mechelen Gent Eupen St Truiden Beerschot VA Oostende Genk Cercle Brugge Standard Waasland-Beveren Oud-Heverlee Leuven Waregem Charleroi Gent Antwerp Kortrijk Anderlecht Mouscron</t>
-  </si>
-  <si>
-    <t>Eupen,Oud-Heverlee Leuven Club Brugge Kortrijk St Truiden Gent Antwerp Anderlecht Cercle Brugge Mouscron Genk Waasland-Beveren Standard Charleroi Mechelen Beerschot VA Club Brugge Waregem Genk Cercle Brugge Oostende Anderlecht Beerschot VA Mechelen Antwerp Mouscron Gent Waasland-Beveren Oostende St Truiden Oud-Heverlee Leuven Kortrijk Waregem Standard Charleroi</t>
-  </si>
-  <si>
-    <t>Genk,Waregem Oud-Heverlee Leuven Standard Club Brugge Beerschot VA Mechelen Oostende Waasland-Beveren Charleroi Gent Eupen St Truiden Mouscron Cercle Brugge Antwerp Anderlecht Kortrijk Waasland-Beveren Eupen Kortrijk Mouscron Gent Club Brugge Waregem Mechelen Anderlecht Oostende Beerschot VA Charleroi Cercle Brugge Standard Oud-Heverlee Leuven St Truiden Antwerp</t>
-  </si>
-  <si>
-    <t>Gent,St Truiden Kortrijk Antwerp Mechelen Eupen Mouscron Oud-Heverlee Leuven Beerschot VA Cercle Brugge Genk Waasland-Beveren Anderlecht Charleroi Waregem Oostende Standard Waasland-Beveren Club Brugge Kortrijk Beerschot VA Antwerp Genk Oud-Heverlee Leuven St Truiden Anderlecht Eupen Mouscron Mechelen Oostende Club Brugge Cercle Brugge Standard Charleroi Waregem</t>
-  </si>
-  <si>
-    <t>Kortrijk,Waasland-Beveren Gent Eupen Cercle Brugge Mouscron Standard Antwerp St Truiden Mechelen Anderlecht Waregem Beerschot VA Club Brugge Oostende Charleroi Oud-Heverlee Leuven Standard Genk Gent Genk Oostende St Truiden Cercle Brugge Beerschot VA Charleroi Mouscron Oud-Heverlee Leuven Anderlecht Waregem Antwerp Eupen Club Brugge Waasland-Beveren Mechelen</t>
-  </si>
-  <si>
-    <t>Mechelen,Anderlecht Mouscron Cercle Brugge Gent Oostende Genk St Truiden Antwerp Kortrijk Club Brugge Charleroi Waregem Beerschot VA Eupen Standard Waasland-Beveren Club Brugge Oud-Heverlee Leuven Mouscron Antwerp Charleroi Standard Eupen Waasland-Beveren Genk Cercle Brugge Beerschot VA Gent Oostende Anderlecht Oud-Heverlee Leuven St Truiden Waregem Kortrijk</t>
-  </si>
-  <si>
-    <t>Mouscron,Antwerp Mechelen Anderlecht Waregem Kortrijk Gent Charleroi Oostende Eupen Genk Cercle Brugge Club Brugge St Truiden Waasland-Beveren Oud-Heverlee Leuven Beerschot VA Oud-Heverlee Leuven Standard Mechelen Waregem Genk Waasland-Beveren St Truiden Anderlecht Eupen Kortrijk Gent Cercle Brugge Beerschot VA Standard Oostende Charleroi Antwerp Club Brugge</t>
-  </si>
-  <si>
-    <t>Oostende,Beerschot VA Charleroi St Truiden Anderlecht Mechelen Oud-Heverlee Leuven Genk Mouscron Waregem Standard Club Brugge Antwerp Waasland-Beveren Kortrijk Gent Cercle Brugge Anderlecht Oud-Heverlee Leuven Charleroi Eupen Kortrijk Club Brugge Antwerp Standard Waregem St Truiden Genk Eupen Mechelen Gent Mouscron Waasland-Beveren Beerschot VA Cercle Brugge</t>
-  </si>
-  <si>
-    <t>Oud-Heverlee Leuven,Eupen Genk Charleroi Waasland-Beveren Standard Oostende Gent Waregem Anderlecht Club Brugge Beerschot VA St Truiden Antwerp Cercle Brugge Mouscron Kortrijk Mouscron Mechelen Oostende Anderlecht St Truiden Waregem Gent Charleroi Beerschot VA Standard Kortrijk Club Brugge Antwerp Eupen Mechelen Genk Cercle Brugge Waasland-Beveren</t>
-  </si>
-  <si>
-    <t>St Truiden,Gent Anderlecht Oostende Eupen Antwerp Cercle Brugge Mechelen Kortrijk Beerschot VA Standard Genk Oud-Heverlee Leuven Waasland-Beveren Mouscron Club Brugge Charleroi Waregem Standard Beerschot VA Club Brugge Oud-Heverlee Leuven Kortrijk Mouscron Gent Cercle Brugge Oostende Waregem Antwerp Eupen Charleroi Mechelen Waasland-Beveren Genk Anderlecht</t>
-  </si>
-  <si>
-    <t>Standard,Cercle Brugge Waasland-Beveren Genk Beerschot VA Oud-Heverlee Leuven Kortrijk Waregem Charleroi Club Brugge St Truiden Oostende Antwerp Eupen Anderlecht Mechelen Gent Kortrijk Mouscron St Truiden Waasland-Beveren Cercle Brugge Mechelen Charleroi Oostende Club Brugge Oud-Heverlee Leuven Antwerp Waregem Anderlecht Mouscron Genk Gent Eupen Beerschot VA</t>
-  </si>
-  <si>
-    <t>Waasland-Beveren,Kortrijk Standard Waregem Oud-Heverlee Leuven Club Brugge Anderlecht Beerschot VA Genk Gent Eupen Cercle Brugge Oostende St Truiden Charleroi Mouscron Mechelen Gent Antwerp Genk Standard Waregem Mouscron Anderlecht Mechelen Antwerp Club Brugge Eupen Charleroi Cercle Brugge Beerschot VA Oostende St Truiden Kortrijk Oud-Heverlee Leuven</t>
-  </si>
-  <si>
-    <t>Waregem,Genk Beerschot VA Waasland-Beveren Mouscron Charleroi Club Brugge Standard Oud-Heverlee Leuven Antwerp Oostende Kortrijk Cercle Brugge Mechelen Gent Anderlecht Antwerp St Truiden Cercle Brugge Eupen Mouscron Waasland-Beveren Oud-Heverlee Leuven Beerschot VA Genk Oostende Charleroi St Truiden Standard Kortrijk Club Brugge Anderlecht Eupen Mechelen Gent</t>
+    <t>Anderlecht,W D W W W W</t>
+  </si>
+  <si>
+    <t>Antwerp,L W W L W W</t>
+  </si>
+  <si>
+    <t>Beerschot VA,D W L W L L</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,W L L W W D</t>
+  </si>
+  <si>
+    <t>Charleroi,D D D L L L</t>
+  </si>
+  <si>
+    <t>Club Brugge,D W L W L W</t>
+  </si>
+  <si>
+    <t>Eupen,W D W L L W</t>
+  </si>
+  <si>
+    <t>Genk,W W D W W L</t>
+  </si>
+  <si>
+    <t>Gent,W L W L W W</t>
+  </si>
+  <si>
+    <t>Kortrijk,L L L L W L</t>
+  </si>
+  <si>
+    <t>Mechelen,L D D L W W</t>
+  </si>
+  <si>
+    <t>Mouscron,D W L D L L</t>
+  </si>
+  <si>
+    <t>Oostende,W L W L W D</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,W D D L L L</t>
+  </si>
+  <si>
+    <t>St Truiden,L D W W L L</t>
+  </si>
+  <si>
+    <t>Standard,L L D W W W</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,L L W L L W</t>
+  </si>
+  <si>
+    <t>Waregem,W L L W L L</t>
+  </si>
+  <si>
+    <t>Anderlecht,3 1 4 4 2 1,(15)</t>
+  </si>
+  <si>
+    <t>Antwerp,0 4 2 1 3 3,(13)</t>
+  </si>
+  <si>
+    <t>Beerschot VA,2 2 1 2 1 0,(8)</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,2 0 0 2 3 1,(8)</t>
+  </si>
+  <si>
+    <t>Charleroi,0 1 1 1 0 2,(5)</t>
+  </si>
+  <si>
+    <t>Club Brugge,1 4 0 2 1 4,(12)</t>
+  </si>
+  <si>
+    <t>Eupen,2 3 2 1 0 3,(11)</t>
+  </si>
+  <si>
+    <t>Genk,2 2 2 3 4 2,(15)</t>
+  </si>
+  <si>
+    <t>Gent,1 0 1 1 4 7,(14)</t>
+  </si>
+  <si>
+    <t>Kortrijk,1 2 0 1 4 1,(9)</t>
+  </si>
+  <si>
+    <t>Mechelen,0 1 2 1 4 4,(12)</t>
+  </si>
+  <si>
+    <t>Mouscron,2 1 0 1 2 2,(8)</t>
+  </si>
+  <si>
+    <t>Oostende,2 0 1 0 2 1,(6)</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,2 3 2 2 0 1,(10)</t>
+  </si>
+  <si>
+    <t>St Truiden,0 0 2 4 0 0,(6)</t>
+  </si>
+  <si>
+    <t>Standard,1 0 2 2 4 3,(12)</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,0 1 2 2 3 2,(10)</t>
+  </si>
+  <si>
+    <t>Waregem,2 0 1 2 2 2,(9)</t>
+  </si>
+  <si>
+    <t>Anderlecht,1 1 1 1 1 0,(5)</t>
+  </si>
+  <si>
+    <t>Antwerp,2 2 0 4 2 2,(12)</t>
+  </si>
+  <si>
+    <t>Beerschot VA,2 1 2 1 2 3,(11)</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,0 2 1 1 0 1,(5)</t>
+  </si>
+  <si>
+    <t>Charleroi,0 1 1 2 4 3,(11)</t>
+  </si>
+  <si>
+    <t>Club Brugge,1 0 2 1 2 2,(8)</t>
+  </si>
+  <si>
+    <t>Eupen,0 3 0 2 4 2,(11)</t>
+  </si>
+  <si>
+    <t>Genk,1 0 2 2 0 3,(8)</t>
+  </si>
+  <si>
+    <t>Gent,0 4 0 2 0 2,(8)</t>
+  </si>
+  <si>
+    <t>Kortrijk,2 4 2 2 3 4,(17)</t>
+  </si>
+  <si>
+    <t>Mechelen,2 1 2 2 2 1,(10)</t>
+  </si>
+  <si>
+    <t>Mouscron,2 0 1 1 3 4,(11)</t>
+  </si>
+  <si>
+    <t>Oostende,0 1 0 2 1 1,(5)</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,0 3 2 3 3 2,(13)</t>
+  </si>
+  <si>
+    <t>St Truiden,2 0 1 2 4 1,(10)</t>
+  </si>
+  <si>
+    <t>Standard,3 1 2 1 0 0,(7)</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,2 2 0 4 4 1,(13)</t>
+  </si>
+  <si>
+    <t>Waregem,1 3 4 1 4 7,(20)</t>
+  </si>
+  <si>
+    <t>Anderlecht,4 2 5 5 3 1,(20)</t>
+  </si>
+  <si>
+    <t>Antwerp,2 6 2 5 5 5,(25)</t>
+  </si>
+  <si>
+    <t>Beerschot VA,4 3 3 3 3 3,(19)</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,2 2 1 3 3 2,(13)</t>
+  </si>
+  <si>
+    <t>Charleroi,0 2 2 3 4 5,(16)</t>
+  </si>
+  <si>
+    <t>Club Brugge,2 4 2 3 3 6,(20)</t>
+  </si>
+  <si>
+    <t>Eupen,2 6 2 3 4 5,(22)</t>
+  </si>
+  <si>
+    <t>Genk,3 2 4 5 4 5,(23)</t>
+  </si>
+  <si>
+    <t>Gent,1 4 1 3 4 9,(22)</t>
+  </si>
+  <si>
+    <t>Kortrijk,3 6 2 3 7 5,(26)</t>
+  </si>
+  <si>
+    <t>Mechelen,2 2 4 3 6 5,(22)</t>
+  </si>
+  <si>
+    <t>Mouscron,4 1 1 2 5 6,(19)</t>
+  </si>
+  <si>
+    <t>Oostende,2 1 1 2 3 2,(11)</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,2 6 4 5 3 3,(23)</t>
+  </si>
+  <si>
+    <t>St Truiden,2 0 3 6 4 1,(16)</t>
+  </si>
+  <si>
+    <t>Standard,4 1 4 3 4 3,(19)</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,2 3 2 6 7 3,(23)</t>
+  </si>
+  <si>
+    <t>Waregem,3 3 5 3 6 9,(29)</t>
+  </si>
+  <si>
+    <t>Anderlecht,Standard Mechelen Waregem Antwerp Club Brugge St Truiden</t>
+  </si>
+  <si>
+    <t>Antwerp,Oud-Heverlee Leuven Kortrijk Club Brugge Anderlecht Mouscron Genk</t>
+  </si>
+  <si>
+    <t>Beerschot VA,Mouscron Waasland-Beveren Cercle Brugge Charleroi Oostende Standard</t>
+  </si>
+  <si>
+    <t>Cercle Brugge,Waasland-Beveren Genk Gent Beerschot VA Oud-Heverlee Leuven Oostende</t>
+  </si>
+  <si>
+    <t>Charleroi,St Truiden Club Brugge Mouscron Beerschot VA Gent Eupen</t>
+  </si>
+  <si>
+    <t>Club Brugge,Charleroi Gent Antwerp Kortrijk Anderlecht Mouscron</t>
+  </si>
+  <si>
+    <t>Eupen,St Truiden Oud-Heverlee Leuven Kortrijk Waregem Standard Charleroi</t>
+  </si>
+  <si>
+    <t>Genk,Charleroi Cercle Brugge Standard Oud-Heverlee Leuven St Truiden Antwerp</t>
+  </si>
+  <si>
+    <t>Gent,Oostende Club Brugge Cercle Brugge Standard Charleroi Waregem</t>
+  </si>
+  <si>
+    <t>Kortrijk,Waregem Antwerp Eupen Club Brugge Waasland-Beveren Mechelen</t>
+  </si>
+  <si>
+    <t>Mechelen,Oostende Anderlecht Oud-Heverlee Leuven St Truiden Waregem Kortrijk</t>
+  </si>
+  <si>
+    <t>Mouscron,Beerschot VA Standard Oostende Charleroi Antwerp Club Brugge</t>
+  </si>
+  <si>
+    <t>Oostende,Mechelen Gent Mouscron Waasland-Beveren Beerschot VA Cercle Brugge</t>
+  </si>
+  <si>
+    <t>Oud-Heverlee Leuven,Antwerp Eupen Mechelen Genk Cercle Brugge Waasland-Beveren</t>
+  </si>
+  <si>
+    <t>St Truiden,Eupen Charleroi Mechelen Waasland-Beveren Genk Anderlecht</t>
+  </si>
+  <si>
+    <t>Standard,Anderlecht Mouscron Genk Gent Eupen Beerschot VA</t>
+  </si>
+  <si>
+    <t>Waasland-Beveren,Cercle Brugge Beerschot VA Oostende St Truiden Kortrijk Oud-Heverlee Leuven</t>
+  </si>
+  <si>
+    <t>Waregem,Kortrijk Club Brugge Anderlecht Eupen Mechelen Gent</t>
   </si>
 </sst>
 </file>
@@ -1501,9 +1501,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -32236,15 +32235,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="23" max="23" width="15.42578125" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -35131,16 +35124,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="89.42578125" customWidth="1"/>
-    <col min="3" max="3" width="72.7109375" customWidth="1"/>
-    <col min="4" max="4" width="74.140625" customWidth="1"/>
-    <col min="5" max="5" width="83" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" customWidth="1"/>
+    <col min="6" max="6" width="94.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -35161,8 +35153,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>390</v>
@@ -35181,8 +35173,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>391</v>
@@ -35201,8 +35193,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>392</v>
@@ -35221,8 +35213,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>393</v>
@@ -35241,8 +35233,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>394</v>
@@ -35261,8 +35253,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>395</v>
@@ -35281,8 +35273,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>396</v>
@@ -35301,8 +35293,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>397</v>
@@ -35321,8 +35313,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>398</v>
@@ -35341,8 +35333,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>399</v>
@@ -35361,8 +35353,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>400</v>
@@ -35381,8 +35373,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>401</v>
@@ -35401,8 +35393,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>402</v>
@@ -35421,8 +35413,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>403</v>
@@ -35441,8 +35433,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>404</v>
@@ -35461,8 +35453,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>405</v>
@@ -35481,8 +35473,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>406</v>
@@ -35501,8 +35493,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>407</v>

</xml_diff>